<commit_message>
update excel and database
</commit_message>
<xml_diff>
--- a/Quiz/quiz.xlsx
+++ b/Quiz/quiz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\C#\Quiz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Intern\Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9AF23A-A581-492C-89C2-FC724C62B472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F532C3-2E49-40F8-B1FC-DA9572EDB2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F94A5F0F-75EB-47CE-A31A-3FD75DDA5E59}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -78,6 +78,132 @@
   </si>
   <si>
     <t>no answer</t>
+  </si>
+  <si>
+    <t>A option</t>
+  </si>
+  <si>
+    <t>B option</t>
+  </si>
+  <si>
+    <t>C option</t>
+  </si>
+  <si>
+    <t>D option</t>
+  </si>
+  <si>
+    <t>Multi choice right&amp;wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Writing</t>
+  </si>
+  <si>
+    <t>Kế thừa</t>
+  </si>
+  <si>
+    <t>Inherite</t>
+  </si>
+  <si>
+    <t>option-Type</t>
+  </si>
+  <si>
+    <t>1InM</t>
+  </si>
+  <si>
+    <t>override</t>
+  </si>
+  <si>
+    <t>ghi đè</t>
+  </si>
+  <si>
+    <t>2InM</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>topic_id</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>advance</t>
+  </si>
+  <si>
+    <t>teo</t>
+  </si>
+  <si>
+    <t>QuizQuestions</t>
+  </si>
+  <si>
+    <t>quiz_id</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>level_id</t>
+  </si>
+  <si>
+    <t>tag_id</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id </t>
+  </si>
+  <si>
+    <t>QuizUser</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>answer_id</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>owner_id</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>quiz_question_id</t>
+  </si>
+  <si>
+    <t>Multi choice</t>
+  </si>
+  <si>
+    <t>dotnet</t>
   </si>
 </sst>
 </file>
@@ -145,24 +271,129 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4C600C3-F691-48CA-82BF-9FA6DD8551DF}" name="Table1" displayName="Table1" ref="A2:D5" totalsRowShown="0">
-  <autoFilter ref="A2:D5" xr:uid="{F4C600C3-F691-48CA-82BF-9FA6DD8551DF}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F4C600C3-F691-48CA-82BF-9FA6DD8551DF}" name="Table1" displayName="Table1" ref="A2:F8" totalsRowShown="0">
+  <autoFilter ref="A2:F8" xr:uid="{F4C600C3-F691-48CA-82BF-9FA6DD8551DF}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{243CC72A-AFC5-4EE3-95E5-74FD54672778}" name="id"/>
     <tableColumn id="2" xr3:uid="{1B2F405E-9AFB-4013-9DC0-1FEC4755B463}" name="title"/>
     <tableColumn id="3" xr3:uid="{C482FCE4-48BD-4962-8BFB-92F9F90F4F2C}" name="content"/>
     <tableColumn id="4" xr3:uid="{CE44118A-B02F-4360-AD95-B3D9F3D08238}" name="type_id"/>
+    <tableColumn id="5" xr3:uid="{6B861EDA-CB62-4667-81EF-4B68D34106F6}" name="level_id"/>
+    <tableColumn id="6" xr3:uid="{1F77D4F4-6DF8-41F2-AEFB-9959D8DE2581}" name="tag_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}" name="Table10" displayName="Table10" ref="N26:S30" totalsRowShown="0">
+  <autoFilter ref="N26:S30" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{9D79ABA7-54A3-4108-BD7F-E1FD140C9918}" name="id"/>
+    <tableColumn id="2" xr3:uid="{BFD3E508-A84A-411E-AAF9-DE5CD8DEE04E}" name="quiz_question_id"/>
+    <tableColumn id="3" xr3:uid="{87FA8F8F-3452-46F8-A743-AFA447DED9FC}" name="user_id"/>
+    <tableColumn id="4" xr3:uid="{5CC8461E-20A7-451D-A967-52AD7D2071AA}" name="answer_id"/>
+    <tableColumn id="5" xr3:uid="{F90A7244-ECE6-4AB5-8748-C79BD525EFDA}" name="score"/>
+    <tableColumn id="7" xr3:uid="{D3F8A565-C78E-4F03-989A-04C6AF288504}" name="result"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A70F0B7-E74F-42D3-A234-884B8C02A1A3}" name="Table2" displayName="Table2" ref="H2:I3" totalsRowShown="0">
-  <autoFilter ref="H2:I3" xr:uid="{2A70F0B7-E74F-42D3-A234-884B8C02A1A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A70F0B7-E74F-42D3-A234-884B8C02A1A3}" name="Table2" displayName="Table2" ref="H2:I6" totalsRowShown="0">
+  <autoFilter ref="H2:I6" xr:uid="{2A70F0B7-E74F-42D3-A234-884B8C02A1A3}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{56ACFA66-0155-4C66-B16A-FC1A47DDA182}" name="id"/>
     <tableColumn id="2" xr3:uid="{E6979CE5-BE09-4761-8585-96669FA0B0FE}" name="name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FF04CC7D-45A6-4012-8897-8CA926CD27DF}" name="Table3" displayName="Table3" ref="A14:E34" totalsRowShown="0">
+  <autoFilter ref="A14:E34" xr:uid="{FF04CC7D-45A6-4012-8897-8CA926CD27DF}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C33F7A8B-6F6E-4904-87C8-18DF5DB9DD04}" name="id"/>
+    <tableColumn id="2" xr3:uid="{EC07AF47-03B2-4757-9F36-4B882FAAFE33}" name="content"/>
+    <tableColumn id="3" xr3:uid="{8F717BA9-2582-4E8D-9D9E-2DBD1D92FE2B}" name="question_id"/>
+    <tableColumn id="4" xr3:uid="{2DB8B941-77FF-42FD-8AAA-0F3DFE7700A3}" name="result"/>
+    <tableColumn id="5" xr3:uid="{CBA66DBD-7B9E-4753-A001-99F287457917}" name="option-Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EF2D4D52-9C3D-4867-B983-57AA2867A2E5}" name="Table4" displayName="Table4" ref="H9:I11" totalsRowShown="0">
+  <autoFilter ref="H9:I11" xr:uid="{EF2D4D52-9C3D-4867-B983-57AA2867A2E5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{822C8DF9-8882-46D3-861B-72880EC21885}" name="id"/>
+    <tableColumn id="2" xr3:uid="{E7BFC7FC-9B86-482D-94B8-11DD40443CB6}" name="title"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4AA2D26B-9021-4CCD-98DC-EADE24E31041}" name="Table5" displayName="Table5" ref="K2:M4" totalsRowShown="0">
+  <autoFilter ref="K2:M4" xr:uid="{4AA2D26B-9021-4CCD-98DC-EADE24E31041}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8C7B1264-E96B-4EE6-901F-618D1891B926}" name="id"/>
+    <tableColumn id="2" xr3:uid="{F3F7E10D-1155-4B89-9959-B3498085ACAF}" name="title"/>
+    <tableColumn id="3" xr3:uid="{79909515-0091-408D-BD58-F6E079CF9258}" name="topic_id"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2E3C80CE-74DE-4418-BA3C-B78FC5285C62}" name="Table6" displayName="Table6" ref="H14:M16" totalsRowShown="0">
+  <autoFilter ref="H14:M16" xr:uid="{2E3C80CE-74DE-4418-BA3C-B78FC5285C62}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BDFE0C1D-2856-4F04-B505-859D7F0DF673}" name="id"/>
+    <tableColumn id="2" xr3:uid="{D03C49EE-B276-44B4-9735-B87D0FA40E04}" name="username"/>
+    <tableColumn id="3" xr3:uid="{923DAEB5-F394-438E-A392-FDBC8AE5CCC4}" name="password"/>
+    <tableColumn id="4" xr3:uid="{042BD084-39E9-4C28-94BB-0D793C75CDFC}" name="salt"/>
+    <tableColumn id="5" xr3:uid="{B9779245-3A35-40B8-9FDF-3D6A565A491D}" name="name"/>
+    <tableColumn id="6" xr3:uid="{EC2F67F8-AE18-4277-AFAA-0E5F56353230}" name="email"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}" name="Table7" displayName="Table7" ref="H26:K29" totalsRowShown="0">
+  <autoFilter ref="H26:K29" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F983299F-0695-4341-B0A7-66848B6D896D}" name="id"/>
+    <tableColumn id="2" xr3:uid="{E961788A-BA83-4B6C-9F66-E24F6B21A169}" name="quiz_id"/>
+    <tableColumn id="3" xr3:uid="{9FE0F030-E048-4ADA-8AE2-191E9A8C7EC2}" name="question_id"/>
+    <tableColumn id="4" xr3:uid="{49DE2D04-459A-47E7-8B91-21C9E036E8BB}" name="score"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{13ED4560-55D9-4931-9285-68EF15BC28DC}" name="Table8" displayName="Table8" ref="O2:P3" totalsRowShown="0">
+  <autoFilter ref="O2:P3" xr:uid="{13ED4560-55D9-4931-9285-68EF15BC28DC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4677D7C4-E444-4FED-804B-BFE91322EAF7}" name="id "/>
+    <tableColumn id="2" xr3:uid="{EE4DA4A4-725A-4207-B262-876B5D5EBEC3}" name="title"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{43EBD389-F8E7-4189-AF91-6A891ED06BFB}" name="Table9" displayName="Table9" ref="Q14:S15" totalsRowShown="0">
+  <autoFilter ref="Q14:S15" xr:uid="{43EBD389-F8E7-4189-AF91-6A891ED06BFB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{579F9BB3-1140-47F3-9BBC-223A11775BE8}" name="id"/>
+    <tableColumn id="2" xr3:uid="{4A8EEE54-E896-49F8-8D66-9943269B8E09}" name="title"/>
+    <tableColumn id="3" xr3:uid="{179B3C92-3721-4C7D-861A-7BB0D41BD9F8}" name="owner_id"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -485,32 +716,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B400B98-08AD-4AEB-AC2C-BC94EE50B75C}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" customWidth="1"/>
+    <col min="19" max="19" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="O1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,14 +774,35 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -546,29 +818,147 @@
       <c r="I3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -581,8 +971,38 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -592,8 +1012,26 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -603,16 +1041,433 @@
       <c r="C16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" t="s">
+        <v>41</v>
+      </c>
+      <c r="N26" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>53</v>
+      </c>
+      <c r="P26" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>48</v>
+      </c>
+      <c r="R26" t="s">
+        <v>41</v>
+      </c>
+      <c r="S26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>30</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>50</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
+      <c r="Q28">
+        <v>4</v>
+      </c>
+      <c r="R28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>10</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>3</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>11</v>
+      </c>
+      <c r="R29">
+        <v>10</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="N30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>12</v>
+      </c>
+      <c r="R30">
+        <v>10</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="10">
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="N25:S25"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="10">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update method check answer
</commit_message>
<xml_diff>
--- a/Quiz/quiz.xlsx
+++ b/Quiz/quiz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Intern\Quiz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9F659A-44B2-427F-BC86-2DE45D572D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014E972D-844E-4DD4-8464-C218BDC9AE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F94A5F0F-75EB-47CE-A31A-3FD75DDA5E59}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -204,6 +193,12 @@
   </si>
   <si>
     <t>dotnet</t>
+  </si>
+  <si>
+    <t>ke thua</t>
+  </si>
+  <si>
+    <t>option-type</t>
   </si>
 </sst>
 </file>
@@ -286,15 +281,17 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}" name="Table10" displayName="Table10" ref="N26:S30" totalsRowShown="0">
-  <autoFilter ref="N26:S30" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}" name="Table10" displayName="Table10" ref="N26:U31" totalsRowShown="0">
+  <autoFilter ref="N26:U31" xr:uid="{27C2180B-10B2-41D7-9867-ACBB9D57ADD6}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D79ABA7-54A3-4108-BD7F-E1FD140C9918}" name="id"/>
     <tableColumn id="2" xr3:uid="{BFD3E508-A84A-411E-AAF9-DE5CD8DEE04E}" name="quiz_question_id"/>
     <tableColumn id="3" xr3:uid="{87FA8F8F-3452-46F8-A743-AFA447DED9FC}" name="user_id"/>
     <tableColumn id="4" xr3:uid="{5CC8461E-20A7-451D-A967-52AD7D2071AA}" name="answer_id"/>
     <tableColumn id="5" xr3:uid="{F90A7244-ECE6-4AB5-8748-C79BD525EFDA}" name="score"/>
     <tableColumn id="7" xr3:uid="{D3F8A565-C78E-4F03-989A-04C6AF288504}" name="result"/>
+    <tableColumn id="6" xr3:uid="{4D3954F7-BC73-4B07-81ED-5E18444E4D60}" name="content"/>
+    <tableColumn id="8" xr3:uid="{17EDE8DC-5B86-427A-B69C-509655FBD26E}" name="option-type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -364,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}" name="Table7" displayName="Table7" ref="H26:K29" totalsRowShown="0">
-  <autoFilter ref="H26:K29" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}" name="Table7" displayName="Table7" ref="H26:K30" totalsRowShown="0">
+  <autoFilter ref="H26:K30" xr:uid="{81AD4BEC-9E3E-41D2-B2A3-DAF5FB6205BD}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F983299F-0695-4341-B0A7-66848B6D896D}" name="id"/>
     <tableColumn id="2" xr3:uid="{E961788A-BA83-4B6C-9F66-E24F6B21A169}" name="quiz_id"/>
@@ -716,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B400B98-08AD-4AEB-AC2C-BC94EE50B75C}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,6 +734,8 @@
     <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.5546875" customWidth="1"/>
     <col min="19" max="19" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -1049,7 +1048,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>6</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1121,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>10</v>
       </c>
@@ -1146,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>11</v>
       </c>
@@ -1173,8 +1172,10 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -1217,8 +1218,14 @@
       <c r="S26" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T26" t="s">
+        <v>2</v>
+      </c>
+      <c r="U26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>15</v>
       </c>
@@ -1341,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1357,6 +1364,18 @@
       <c r="E30" t="s">
         <v>23</v>
       </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>30</v>
+      </c>
       <c r="N30">
         <v>3</v>
       </c>
@@ -1376,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1392,8 +1411,29 @@
       <c r="E31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>4</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <v>30</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>56</v>
+      </c>
+      <c r="U31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1454,8 +1494,8 @@
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q13:S13"/>
-    <mergeCell ref="N25:S25"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="N25:U25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="10">

</xml_diff>